<commit_message>
corrige flujo luego de ingreso patente manual
</commit_message>
<xml_diff>
--- a/archivo.xlsx
+++ b/archivo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="85">
   <si>
     <t>Columna_1</t>
   </si>
@@ -37,70 +37,238 @@
     <t>Columna_7</t>
   </si>
   <si>
-    <t>95748</t>
-  </si>
-  <si>
-    <t>95642</t>
-  </si>
-  <si>
-    <t>95730</t>
-  </si>
-  <si>
-    <t>95698</t>
-  </si>
-  <si>
-    <t>95723</t>
-  </si>
-  <si>
-    <t>95733</t>
-  </si>
-  <si>
-    <t>95699</t>
+    <t>95656</t>
+  </si>
+  <si>
+    <t>95722</t>
+  </si>
+  <si>
+    <t>95676</t>
+  </si>
+  <si>
+    <t>95618</t>
+  </si>
+  <si>
+    <t>95671</t>
+  </si>
+  <si>
+    <t>95644</t>
+  </si>
+  <si>
+    <t>95692</t>
+  </si>
+  <si>
+    <t>95672</t>
+  </si>
+  <si>
+    <t>95663</t>
+  </si>
+  <si>
+    <t>95675</t>
+  </si>
+  <si>
+    <t>95678</t>
+  </si>
+  <si>
+    <t>95669</t>
+  </si>
+  <si>
+    <t>95679</t>
+  </si>
+  <si>
+    <t>95702</t>
+  </si>
+  <si>
+    <t>95660</t>
+  </si>
+  <si>
+    <t>95651</t>
+  </si>
+  <si>
+    <t>95712</t>
+  </si>
+  <si>
+    <t>95629</t>
+  </si>
+  <si>
+    <t>95654</t>
   </si>
   <si>
     <t>-pat</t>
   </si>
   <si>
-    <t>AB895RT</t>
-  </si>
-  <si>
-    <t>AF941DJ</t>
-  </si>
-  <si>
-    <t>AD795OU</t>
-  </si>
-  <si>
-    <t>PER655</t>
-  </si>
-  <si>
-    <t>AC166NO</t>
-  </si>
-  <si>
-    <t>AE498DY</t>
-  </si>
-  <si>
-    <t>AA969PZ</t>
+    <t>HYE282</t>
+  </si>
+  <si>
+    <t>NHO427</t>
+  </si>
+  <si>
+    <t>EUZ030</t>
+  </si>
+  <si>
+    <t>AF910UV</t>
+  </si>
+  <si>
+    <t>BAY557</t>
+  </si>
+  <si>
+    <t>AC419SL</t>
+  </si>
+  <si>
+    <t>IDK425</t>
+  </si>
+  <si>
+    <t>AA303RO</t>
+  </si>
+  <si>
+    <t>IIA343</t>
+  </si>
+  <si>
+    <t>AD762LL</t>
+  </si>
+  <si>
+    <t>AE824WO</t>
+  </si>
+  <si>
+    <t>PCJ114</t>
+  </si>
+  <si>
+    <t>AG781KA</t>
+  </si>
+  <si>
+    <t>AF383EN</t>
+  </si>
+  <si>
+    <t>AB033CS</t>
+  </si>
+  <si>
+    <t>AG095MM</t>
+  </si>
+  <si>
+    <t>AB555WU</t>
+  </si>
+  <si>
+    <t>AB859OT</t>
+  </si>
+  <si>
+    <t>HNE508</t>
   </si>
   <si>
     <t>-pol</t>
   </si>
   <si>
-    <t>-ord</t>
-  </si>
-  <si>
-    <t>6040098804701</t>
-  </si>
-  <si>
-    <t>5056085</t>
-  </si>
-  <si>
-    <t>5054842</t>
+    <t>7182118</t>
+  </si>
+  <si>
+    <t>10755442</t>
+  </si>
+  <si>
+    <t>4-66190007</t>
+  </si>
+  <si>
+    <t>10553759</t>
+  </si>
+  <si>
+    <t>6040093144010</t>
+  </si>
+  <si>
+    <t>10787442</t>
+  </si>
+  <si>
+    <t>8070302002611</t>
+  </si>
+  <si>
+    <t>6040094330008</t>
+  </si>
+  <si>
+    <t>10764439</t>
+  </si>
+  <si>
+    <t>10794218</t>
+  </si>
+  <si>
+    <t>6040091704312</t>
+  </si>
+  <si>
+    <t>10766426</t>
+  </si>
+  <si>
+    <t>10634911</t>
+  </si>
+  <si>
+    <t>6040093137107</t>
+  </si>
+  <si>
+    <t>2398166</t>
+  </si>
+  <si>
+    <t>57704189</t>
+  </si>
+  <si>
+    <t>7313966</t>
+  </si>
+  <si>
+    <t>6040098565602</t>
+  </si>
+  <si>
+    <t>40-0250747-02</t>
   </si>
   <si>
     <t>-sin</t>
   </si>
   <si>
-    <t>60400009630</t>
+    <t>1100657</t>
+  </si>
+  <si>
+    <t>2369024</t>
+  </si>
+  <si>
+    <t>4-3311234</t>
+  </si>
+  <si>
+    <t>2362900</t>
+  </si>
+  <si>
+    <t>60407091780</t>
+  </si>
+  <si>
+    <t>2367806</t>
+  </si>
+  <si>
+    <t>84390090979</t>
+  </si>
+  <si>
+    <t>60407091771</t>
+  </si>
+  <si>
+    <t>2368118</t>
+  </si>
+  <si>
+    <t>2368243</t>
+  </si>
+  <si>
+    <t>60407091755</t>
+  </si>
+  <si>
+    <t>2368202</t>
+  </si>
+  <si>
+    <t>2368350</t>
+  </si>
+  <si>
+    <t>60400009472</t>
+  </si>
+  <si>
+    <t>707836</t>
+  </si>
+  <si>
+    <t>2910530</t>
+  </si>
+  <si>
+    <t>1101133</t>
+  </si>
+  <si>
+    <t>60407091638</t>
   </si>
 </sst>
 </file>
@@ -458,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -492,10 +660,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -503,22 +683,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -526,16 +706,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -543,10 +729,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -554,10 +752,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -565,16 +775,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>52</v>
+      </c>
+      <c r="F7" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -582,10 +798,292 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
         <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>